<commit_message>
added single info line in Logger
</commit_message>
<xml_diff>
--- a/heart_failure/results/df/test_log.xlsx
+++ b/heart_failure/results/df/test_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>n_features</t>
+          <t>added_features</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -478,6 +478,11 @@
       <c r="D2" t="b">
         <v>0</v>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>['age', 'sex']</t>
+        </is>
+      </c>
       <c r="F2" t="n">
         <v>0.66</v>
       </c>
@@ -498,11 +503,165 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>['age', 'sex', 'ponytail']</t>
+        </is>
+      </c>
       <c r="F3" t="n">
         <v>0.66</v>
       </c>
       <c r="G3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['age', 'sex']</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['age', 'sex']</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G5" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['age', 'sex']</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>['age', 'sex', 'ponytail']</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>['age', 'sex']</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G8" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" t="n">
+        <v>12</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>['age', 'sex']</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G9" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
models and logger properly working to save and log results; jupyter notebook is a mess, but it's gonna become cleaner now that saving&logging are working
</commit_message>
<xml_diff>
--- a/heart_failure/results/df/test_log.xlsx
+++ b/heart_failure/results/df/test_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>forced_features</t>
+          <t>features</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -462,6 +462,11 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>robustness_iterations</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>results_df</t>
         </is>
       </c>
     </row>
@@ -480,7 +485,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['age', 'sex']</t>
+          <t>['age', 'anaemia', 'creatinine_phosphokinase', 'diabetes', 'ejection_fraction', 'high_blood_pressure', 'platelets', 'serum_creatinine', 'serum_sodium', 'sex', 'smoking']</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -488,6 +493,11 @@
       </c>
       <c r="G2" t="n">
         <v>100</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>df0</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -501,11 +511,11 @@
         <v>0</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['age', 'sex', 'ponytail']</t>
+          <t>['age', 'anaemia', 'creatinine_phosphokinase', 'diabetes', 'ejection_fraction', 'high_blood_pressure', 'platelets', 'serum_creatinine', 'serum_sodium', 'sex', 'smoking']</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -513,6 +523,11 @@
       </c>
       <c r="G3" t="n">
         <v>100</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>df1</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -520,17 +535,17 @@
         <v>0</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['age', 'sex']</t>
+          <t>['age', 'anaemia', 'creatinine_phosphokinase', 'diabetes', 'ejection_fraction', 'high_blood_pressure', 'platelets', 'serum_creatinine', 'serum_sodium', 'sex', 'smoking']</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -538,6 +553,11 @@
       </c>
       <c r="G4" t="n">
         <v>100</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>df2</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -545,17 +565,17 @@
         <v>0</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="n">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['age', 'sex']</t>
+          <t>['age', 'anaemia', 'creatinine_phosphokinase', 'diabetes', 'ejection_fraction', 'high_blood_pressure', 'platelets', 'serum_creatinine', 'serum_sodium', 'sex', 'smoking']</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -564,105 +584,10 @@
       <c r="G5" t="n">
         <v>100</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>['age', 'sex']</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="G6" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>['age', 'sex', 'ponytail']</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="G7" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>10</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>['age', 'sex']</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="G8" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" t="n">
-        <v>12</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>['age', 'sex']</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="G9" t="n">
-        <v>100</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>df3</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>